<commit_message>
Add Test cases for Password 1
</commit_message>
<xml_diff>
--- a/Choice_Stationery_Supplies_Test_cases_Login_Page_Password.xlsx
+++ b/Choice_Stationery_Supplies_Test_cases_Login_Page_Password.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <r>
       <rPr>
@@ -121,18 +121,6 @@
 "Password" field</t>
   </si>
   <si>
-    <t>TC_Pass_03</t>
-  </si>
-  <si>
-    <t>Verify the minimum  length accepted in the "Password" field</t>
-  </si>
-  <si>
-    <t>TC_Pass_04</t>
-  </si>
-  <si>
-    <t>Verify the maximum  length accepted in the "Password" field</t>
-  </si>
-  <si>
     <t>OS: Windows 10 Enterprise LTSC (64 bit operating system, x64 processor), version 1809, OS build 17763.1217
 Google Chrome v. 114.0.5735.134
 (Official build), (64 bit)</t>
@@ -160,48 +148,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>URL:  https://www.choicestationery.com/
-Email:xxxxxxxxx@gmail.com
-Password value: 1</t>
-  </si>
-  <si>
-    <t>URL:  https://www.choicestationery.com/
-Email:xxxxxxxxx@gmail.com
-Password value:  (∞)</t>
-  </si>
-  <si>
-    <t>1.Open Browser 
-2.Open URL
-3.Go to the Login page
-4.Enter the Email value in the Email field
-5.Enter password value in the password field
-6.Click  the login button</t>
-  </si>
-  <si>
-    <t>1.Open Browser 
-2.Open URL
-3.Go to the Login page
-4.Enter the Email value in the Email field
-5.Enter the password  value in the password field
-6.Click  the Login button</t>
-  </si>
-  <si>
-    <t>1.The browser is opened
-2.Ecommerce website is opened
-3.The login page is opened
-4.The Email value is displayed  in the Email field
-5. The password value  is displayed in the password field and a pop-up window notifies us of the minimum value allowed.
-6.A pop-up window notifies us about the minimum allowed value and the false password.</t>
-  </si>
-  <si>
-    <t>1.The browser is opened
-2.Ecommerce website is opened
-3.The login page is opened
-4.The Email value is displayed in the Email field
-5. The password value  is displayed in the password field and a pop-up window notifies us of the maximum value allowed.
-6.A pop-up window notifies us about the maximum allowed value and the false password.</t>
   </si>
   <si>
     <t xml:space="preserve">1.Open Browser 
@@ -217,60 +163,12 @@
 4.The placeholder is displayed in the "Password" field
 </t>
   </si>
-  <si>
-    <r>
-      <t>Failed.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The placholder is not displayed in the 
-"Password" field</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Failed. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nothing notifies us
-about the acceptability of the minimum length</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Failed. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nothing notifies us
-about the acceptability of the maximum length</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,20 +242,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -436,21 +320,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -732,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,33 +672,33 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,70 +744,38 @@
         <v>16</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>45</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -947,7 +784,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -956,26 +793,6 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>